<commit_message>
radar icon fix rare tool
</commit_message>
<xml_diff>
--- a/gu_in/Item.edf/34_RadarItem/RadarItem.xlsx
+++ b/gu_in/Item.edf/34_RadarItem/RadarItem.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650D0802-BAE4-4C32-B0FE-2487CD41F22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B43326-0E6C-44F5-94B1-8FA527D584FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3315" yWindow="1455" windowWidth="18480" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RadarItem" sheetId="1" r:id="rId1"/>
@@ -273,19 +273,19 @@
     <t>Radar that displays the location of all races normal/archon characters.</t>
   </si>
   <si>
-    <t>A20D01</t>
-  </si>
-  <si>
     <t>11111000</t>
   </si>
   <si>
-    <t>A20D02</t>
-  </si>
-  <si>
-    <t>A20D03</t>
-  </si>
-  <si>
     <t>Translation</t>
+  </si>
+  <si>
+    <t>A21401</t>
+  </si>
+  <si>
+    <t>A21402</t>
+  </si>
+  <si>
+    <t>A21403</t>
   </si>
 </sst>
 </file>
@@ -377,9 +377,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -417,9 +417,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -452,9 +452,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -487,9 +504,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -666,55 +700,55 @@
   <dimension ref="A1:AL8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AH11" sqref="AH11"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -830,7 +864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -944,7 +978,7 @@
       </c>
       <c r="AL2" s="2"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
@@ -952,7 +986,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -967,7 +1001,7 @@
         <v>300</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I3" s="3">
         <v>300</v>
@@ -1059,7 +1093,7 @@
       </c>
       <c r="AL3" s="2"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>45</v>
       </c>
@@ -1067,7 +1101,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D4" s="3">
         <v>2</v>
@@ -1082,7 +1116,7 @@
         <v>300</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I4" s="3">
         <v>300</v>
@@ -1174,7 +1208,7 @@
       </c>
       <c r="AL4" s="2"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>47</v>
       </c>
@@ -1182,7 +1216,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D5" s="3">
         <v>3</v>
@@ -1197,7 +1231,7 @@
         <v>300</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I5" s="3">
         <v>300</v>
@@ -1289,7 +1323,7 @@
       </c>
       <c r="AL5" s="2"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>49</v>
       </c>
@@ -1297,7 +1331,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
@@ -1312,7 +1346,7 @@
         <v>300</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I6" s="3">
         <v>300</v>
@@ -1404,7 +1438,7 @@
       </c>
       <c r="AL6" s="2"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1412,7 +1446,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
@@ -1427,7 +1461,7 @@
         <v>300</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I7" s="3">
         <v>300</v>
@@ -1519,7 +1553,7 @@
       </c>
       <c r="AL7" s="2"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>51</v>
       </c>
@@ -1527,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D8" s="3">
         <v>3</v>
@@ -1542,7 +1576,7 @@
         <v>300</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I8" s="3">
         <v>300</v>
@@ -1651,45 +1685,45 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="31" max="33" width="8" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1817,7 +1851,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>RadarItem!A2</f>
         <v>Code</v>
@@ -1967,7 +2001,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>RadarItem!A3</f>
         <v>rdaaa01</v>
@@ -1978,7 +2012,7 @@
       </c>
       <c r="C3" s="1" t="str">
         <f>RadarItem!C3</f>
-        <v>A20D01</v>
+        <v>A21401</v>
       </c>
       <c r="D3">
         <f>RadarItem!D3</f>
@@ -2117,7 +2151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>RadarItem!A4</f>
         <v>rdaaa02</v>
@@ -2128,7 +2162,7 @@
       </c>
       <c r="C4" s="1" t="str">
         <f>RadarItem!C4</f>
-        <v>A20D02</v>
+        <v>A21402</v>
       </c>
       <c r="D4">
         <f>RadarItem!D4</f>
@@ -2267,7 +2301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>RadarItem!A5</f>
         <v>rdaaa03</v>
@@ -2278,7 +2312,7 @@
       </c>
       <c r="C5" s="1" t="str">
         <f>RadarItem!C5</f>
-        <v>A20D03</v>
+        <v>A21403</v>
       </c>
       <c r="D5">
         <f>RadarItem!D5</f>
@@ -2417,7 +2451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>RadarItem!A6</f>
         <v>rdpvp01</v>
@@ -2428,7 +2462,7 @@
       </c>
       <c r="C6" s="1" t="str">
         <f>RadarItem!C6</f>
-        <v>A20D01</v>
+        <v>A21401</v>
       </c>
       <c r="D6">
         <f>RadarItem!D6</f>
@@ -2567,7 +2601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>RadarItem!A7</f>
         <v>rdpvp02</v>
@@ -2578,7 +2612,7 @@
       </c>
       <c r="C7" s="1" t="str">
         <f>RadarItem!C7</f>
-        <v>A20D02</v>
+        <v>A21402</v>
       </c>
       <c r="D7">
         <f>RadarItem!D7</f>
@@ -2717,7 +2751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>RadarItem!A8</f>
         <v>rdpvp03</v>
@@ -2728,7 +2762,7 @@
       </c>
       <c r="C8" s="1" t="str">
         <f>RadarItem!C8</f>
-        <v>A20D03</v>
+        <v>A21403</v>
       </c>
       <c r="D8">
         <f>RadarItem!D8</f>
@@ -2882,9 +2916,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2895,7 +2929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -2904,7 +2938,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>0</v>
       </c>
@@ -2913,7 +2947,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -2922,7 +2956,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -2931,12 +2965,12 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>